<commit_message>
Added CO PLO datasheet
</commit_message>
<xml_diff>
--- a/DataSheets/course.xlsx
+++ b/DataSheets/course.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\xampp\htdocs\Project_REDSight_DBMS_GROUP_1\DataSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Project_REDSight_DBMS_GROUP_1\DataSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7278C2F1-7F97-493F-A7E3-E9565A977214}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A07A59C-A398-46A2-A391-1D0A64EFC05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{45C0E8D6-B45C-4F58-8F64-0C9D44AE474B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="126">
   <si>
     <t>CourseID</t>
   </si>
@@ -77,42 +77,6 @@
     <t xml:space="preserve">Microprocessor, Interfacing and Assembly Language </t>
   </si>
   <si>
-    <t xml:space="preserve">Database Management </t>
-  </si>
-  <si>
-    <t xml:space="preserve">System Analysis and Design </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Web Applications and Internet </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electronics II </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Compiler Construction </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Design of Operating System </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Communication and Computer Networks </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Numerical Methods </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAT 203 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Linear Algebra: Vectors and Matrices </t>
-  </si>
-  <si>
-    <t xml:space="preserve">MAT 301 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ordinary Differential Equations </t>
-  </si>
-  <si>
     <t xml:space="preserve">Electrical Circuit Analysis </t>
   </si>
   <si>
@@ -146,18 +110,6 @@
     <t xml:space="preserve">CSE214 </t>
   </si>
   <si>
-    <t xml:space="preserve">CSE307 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSE309 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSE313 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">CSE315 </t>
-  </si>
-  <si>
     <t>CSE210</t>
   </si>
   <si>
@@ -198,42 +150,6 @@
   </si>
   <si>
     <t>Microprocessor, Interfacing and Assembly Language Lab</t>
-  </si>
-  <si>
-    <t>CSE303</t>
-  </si>
-  <si>
-    <t>CSE303L</t>
-  </si>
-  <si>
-    <t>Database Management Lab</t>
-  </si>
-  <si>
-    <t>CSE310</t>
-  </si>
-  <si>
-    <t>CSE310L</t>
-  </si>
-  <si>
-    <t>Electronics II Lab</t>
-  </si>
-  <si>
-    <t>CSE316</t>
-  </si>
-  <si>
-    <t>CSE316L</t>
-  </si>
-  <si>
-    <t>Data Communication and Computer Networks Lab</t>
-  </si>
-  <si>
-    <t>CSE317</t>
-  </si>
-  <si>
-    <t>CSE317L</t>
-  </si>
-  <si>
-    <t>Numerical Methods Lab</t>
   </si>
   <si>
     <t>          Electrical Circuit I</t>
@@ -504,19 +420,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Biome"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -541,7 +451,7 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -858,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A569DFA1-FE8D-4969-A877-C88B17F78045}">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B74" sqref="B74"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -888,35 +798,35 @@
     </row>
     <row r="2" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>30</v>
+        <v>18</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C2" s="1">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>27</v>
+        <v>15</v>
       </c>
       <c r="C3" s="1">
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>31</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>5</v>
@@ -925,12 +835,12 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>32</v>
+        <v>20</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>6</v>
@@ -939,26 +849,26 @@
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="C6" s="1">
         <v>1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>7</v>
@@ -967,26 +877,26 @@
         <v>3</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>17</v>
       </c>
       <c r="C8" s="1">
         <v>1</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>8</v>
@@ -995,26 +905,26 @@
         <v>3</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C10" s="1">
         <v>1</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>9</v>
@@ -1023,26 +933,26 @@
         <v>3</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="C12" s="1">
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>10</v>
@@ -1051,26 +961,26 @@
         <v>3</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>48</v>
+        <v>32</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="C14" s="1">
         <v>1</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>11</v>
@@ -1079,12 +989,12 @@
         <v>3</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>51</v>
+        <v>35</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>12</v>
@@ -1093,848 +1003,585 @@
         <v>3</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>52</v>
+        <v>36</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>53</v>
+        <v>37</v>
       </c>
       <c r="C17" s="1">
         <v>1</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="C18" s="1">
         <v>3</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="1">
+        <v>3</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C20" s="1">
         <v>3</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="C21" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="C22" s="1">
         <v>3</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="C23" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="C24" s="1">
         <v>3</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="C25" s="1">
         <v>3</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="C26" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="C27" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>20</v>
+        <v>73</v>
       </c>
       <c r="C28" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>64</v>
+        <v>74</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="C29" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="C30" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>23</v>
+        <v>79</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>24</v>
+        <v>80</v>
       </c>
       <c r="C31" s="1">
         <v>3</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>26</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="C32" s="1">
         <v>3</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>67</v>
+        <v>83</v>
       </c>
       <c r="C33" s="1">
         <v>3</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C34" s="1">
         <v>3</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="C35" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>71</v>
+        <v>91</v>
       </c>
       <c r="C36" s="1">
         <v>3</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>72</v>
+        <v>93</v>
       </c>
       <c r="C37" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>73</v>
+        <v>96</v>
       </c>
       <c r="C38" s="1">
         <v>3</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>82</v>
+        <v>98</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>74</v>
+        <v>97</v>
       </c>
       <c r="C39" s="1">
         <v>3</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>84</v>
+        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>75</v>
+        <v>4</v>
       </c>
       <c r="C40" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>84</v>
+        <v>105</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>89</v>
+        <v>102</v>
       </c>
       <c r="C41" s="1">
         <v>3</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="C42" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="C43" s="1">
         <v>3</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="C44" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>96</v>
+        <v>110</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="C45" s="1">
         <v>3</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>93</v>
+        <v>118</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
       <c r="C46" s="1">
         <v>3</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="C47" s="1">
         <v>3</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>99</v>
+        <v>116</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="C48" s="1">
         <v>1</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>105</v>
+        <v>119</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>103</v>
+        <v>121</v>
       </c>
       <c r="C49" s="1">
         <v>3</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="C50" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>107</v>
+        <v>124</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
       <c r="C51" s="1">
         <v>3</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>113</v>
+        <v>65</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>110</v>
+        <v>57</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>109</v>
+        <v>61</v>
       </c>
       <c r="C52" s="1">
         <v>3</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>113</v>
+        <v>65</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>112</v>
+        <v>58</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>111</v>
+        <v>62</v>
       </c>
       <c r="C53" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>113</v>
+        <v>65</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>114</v>
+        <v>59</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>115</v>
+        <v>64</v>
       </c>
       <c r="C54" s="1">
         <v>3</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>127</v>
+        <v>65</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>116</v>
+        <v>60</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>117</v>
+        <v>63</v>
       </c>
       <c r="C55" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>127</v>
+        <v>65</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>119</v>
+        <v>66</v>
       </c>
       <c r="C56" s="1">
         <v>3</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>127</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>120</v>
+        <v>69</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>121</v>
+        <v>67</v>
       </c>
       <c r="C57" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="C58" s="1">
-        <v>3</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="C59" s="1">
-        <v>3</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C60" s="1">
-        <v>3</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C61" s="1">
-        <v>3</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C62" s="1">
-        <v>3</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="C63" s="1">
-        <v>3</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="C64" s="1">
-        <v>3</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="C65" s="1">
-        <v>3</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="C66" s="1">
-        <v>3</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="C67" s="1">
-        <v>3</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C68" s="1">
-        <v>1</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C69" s="1">
-        <v>3</v>
-      </c>
-      <c r="D69" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="C70" s="1">
-        <v>3</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="C71" s="1">
-        <v>3</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A4" r:id="rId1" display="http://www.cse.iub.edu.bd/courses/31" xr:uid="{16762BAC-721D-40DF-8C00-97A27722614B}"/>
-    <hyperlink ref="B4" r:id="rId2" display="http://www.cse.iub.edu.bd/courses/31" xr:uid="{331FBB5B-20C9-4189-B953-6411A551AFAD}"/>
-    <hyperlink ref="A6" r:id="rId3" display="http://www.cse.iub.edu.bd/courses/32" xr:uid="{53C30A30-B630-4B76-AA22-9D3E54C975D4}"/>
-    <hyperlink ref="B6" r:id="rId4" display="http://www.cse.iub.edu.bd/courses/32" xr:uid="{F7F1AA28-090C-490C-8B77-1A0EAE864A96}"/>
-    <hyperlink ref="A8" r:id="rId5" display="http://www.cse.iub.edu.bd/courses/33" xr:uid="{6CF9D084-9B7A-43FD-87B5-344504A26381}"/>
-    <hyperlink ref="B8" r:id="rId6" display="http://www.cse.iub.edu.bd/courses/33" xr:uid="{D28F803C-9750-4219-B5A0-FDFB0B48CD4F}"/>
-    <hyperlink ref="A10" r:id="rId7" display="http://www.cse.iub.edu.bd/courses/35" xr:uid="{9996CBC1-F766-466D-802C-5C6E06E7DD22}"/>
-    <hyperlink ref="B10" r:id="rId8" display="http://www.cse.iub.edu.bd/courses/35" xr:uid="{41386115-4326-439A-814E-A2B711417230}"/>
-    <hyperlink ref="A12" r:id="rId9" display="http://www.cse.iub.edu.bd/courses/36" xr:uid="{E4DBADE5-C0AD-4529-A021-8AED8D944275}"/>
-    <hyperlink ref="B12" r:id="rId10" display="http://www.cse.iub.edu.bd/courses/36" xr:uid="{21C660CD-EFAF-4BDC-993F-9B3E3A0914D3}"/>
-    <hyperlink ref="A14" r:id="rId11" display="http://www.cse.iub.edu.bd/courses/37" xr:uid="{83780686-3E88-4493-973F-328B6E51F764}"/>
-    <hyperlink ref="B14" r:id="rId12" display="http://www.cse.iub.edu.bd/courses/37" xr:uid="{5B5F623A-4F06-4507-8E13-3D6B3EA08607}"/>
-    <hyperlink ref="A15" r:id="rId13" display="http://www.cse.iub.edu.bd/courses/38" xr:uid="{AA77E621-BF7F-4A83-BAAD-6E183A9BDEB0}"/>
-    <hyperlink ref="B15" r:id="rId14" display="http://www.cse.iub.edu.bd/courses/38" xr:uid="{73978803-9308-4504-A56A-E4EEE44C638D}"/>
-    <hyperlink ref="A17" r:id="rId15" display="http://www.cse.iub.edu.bd/courses/39" xr:uid="{49523534-C7E4-4737-840E-170A233182E7}"/>
-    <hyperlink ref="B17" r:id="rId16" display="http://www.cse.iub.edu.bd/courses/39" xr:uid="{FC850A20-0A72-4C12-831B-961393CFCC11}"/>
-    <hyperlink ref="A19" r:id="rId17" display="http://www.cse.iub.edu.bd/courses/40" xr:uid="{32B84FBD-F9F0-4BB5-95B1-4237EA819B94}"/>
-    <hyperlink ref="B19" r:id="rId18" display="http://www.cse.iub.edu.bd/courses/40" xr:uid="{4C1F74B9-4C26-4523-80C3-83A8F00AE60C}"/>
-    <hyperlink ref="A20" r:id="rId19" display="http://www.cse.iub.edu.bd/courses/41" xr:uid="{8611E965-D8D7-4E13-ADE4-965386B40E39}"/>
-    <hyperlink ref="B20" r:id="rId20" display="http://www.cse.iub.edu.bd/courses/41" xr:uid="{7E10B867-0E71-4052-BA24-E1209D82F210}"/>
-    <hyperlink ref="A21" r:id="rId21" display="http://www.cse.iub.edu.bd/courses/42" xr:uid="{ED6F055D-5B33-491C-AC10-B2AA320E3D2C}"/>
-    <hyperlink ref="B21" r:id="rId22" display="http://www.cse.iub.edu.bd/courses/42" xr:uid="{C065A3FD-B166-47C6-B317-1B7005130AA4}"/>
-    <hyperlink ref="A23" r:id="rId23" display="http://www.cse.iub.edu.bd/courses/43" xr:uid="{12AC500D-A006-45D7-9902-FE303CA8706F}"/>
-    <hyperlink ref="B23" r:id="rId24" display="http://www.cse.iub.edu.bd/courses/43" xr:uid="{0169478D-5A9F-4A9E-98EE-26E98C7885C2}"/>
-    <hyperlink ref="A24" r:id="rId25" display="http://www.cse.iub.edu.bd/courses/44" xr:uid="{BA8F0C60-A43F-484F-A692-2DCD24BD4E31}"/>
-    <hyperlink ref="B24" r:id="rId26" display="http://www.cse.iub.edu.bd/courses/44" xr:uid="{CD3CD92E-815F-4E2F-BFFF-B87E520005FF}"/>
-    <hyperlink ref="A25" r:id="rId27" display="http://www.cse.iub.edu.bd/courses/45" xr:uid="{46CA333B-7EC8-4C89-ACE0-F1C35C745EC3}"/>
-    <hyperlink ref="B25" r:id="rId28" display="http://www.cse.iub.edu.bd/courses/45" xr:uid="{86002640-9175-4403-9A26-6C92ADF37AB0}"/>
-    <hyperlink ref="A27" r:id="rId29" display="http://www.cse.iub.edu.bd/courses/46" xr:uid="{5CFD6287-21D8-45B4-929D-21EBE6BBCD63}"/>
-    <hyperlink ref="B27" r:id="rId30" display="http://www.cse.iub.edu.bd/courses/46" xr:uid="{D117C5A2-BF60-4581-A29E-D2D3D2D23EBA}"/>
-    <hyperlink ref="A29" r:id="rId31" display="http://www.cse.iub.edu.bd/courses/47" xr:uid="{39986D2C-002A-4A31-8D8C-85885D781040}"/>
-    <hyperlink ref="B29" r:id="rId32" display="http://www.cse.iub.edu.bd/courses/47" xr:uid="{A65A346B-F729-40E8-8C2B-3CC01DF067D1}"/>
-    <hyperlink ref="A30" r:id="rId33" display="http://www.cse.iub.edu.bd/courses/247" xr:uid="{4254E8EC-5704-427C-895F-418313756D8F}"/>
-    <hyperlink ref="B30" r:id="rId34" display="http://www.cse.iub.edu.bd/courses/247" xr:uid="{B8323FF9-27E6-4857-89F4-13E678BA414B}"/>
-    <hyperlink ref="A31" r:id="rId35" display="http://www.cse.iub.edu.bd/courses/378" xr:uid="{25D94A2C-20E2-4C51-8443-F459325D2A20}"/>
-    <hyperlink ref="B31" r:id="rId36" display="http://www.cse.iub.edu.bd/courses/378" xr:uid="{1DF030A4-DEAB-4D8B-9A81-80CC8C570803}"/>
-    <hyperlink ref="A3" r:id="rId37" display="http://www.cse.iub.edu.bd/courses/30" xr:uid="{8E43E033-2B5D-4E16-92C2-A7DEB0884A95}"/>
-    <hyperlink ref="B3" r:id="rId38" display="http://www.cse.iub.edu.bd/courses/30" xr:uid="{009FA0FF-7AC4-41D9-B360-6714600D6D6B}"/>
-    <hyperlink ref="A2" r:id="rId39" display="http://www.cse.iub.edu.bd/courses/30" xr:uid="{0DC4E93C-81D3-41CC-9BA6-E77BE70FE4FB}"/>
-    <hyperlink ref="B2" r:id="rId40" display="http://www.cse.iub.edu.bd/courses/30" xr:uid="{ABBD4A34-C93E-4B6B-AD35-E26954CE5BF2}"/>
-    <hyperlink ref="A5" r:id="rId41" display="http://www.cse.iub.edu.bd/courses/32" xr:uid="{C9227C30-2E0E-481A-A4A3-BBD9FF99046C}"/>
-    <hyperlink ref="B5" r:id="rId42" display="http://www.cse.iub.edu.bd/courses/32" xr:uid="{7FF9D83C-DBA5-4648-8F56-A43D03E76300}"/>
-    <hyperlink ref="A7" r:id="rId43" display="http://www.cse.iub.edu.bd/courses/33" xr:uid="{1BE96F19-CF37-42AD-8290-65B6135B4605}"/>
-    <hyperlink ref="B7" r:id="rId44" display="http://www.cse.iub.edu.bd/courses/33" xr:uid="{4509D636-6FBE-4BBD-B4D1-2CE356C493FA}"/>
-    <hyperlink ref="A9" r:id="rId45" display="http://www.cse.iub.edu.bd/courses/35" xr:uid="{ABFDD878-9B51-4F87-BBF6-2302A5AE8935}"/>
-    <hyperlink ref="B9" r:id="rId46" display="http://www.cse.iub.edu.bd/courses/35" xr:uid="{A89F98E9-986D-453D-B440-F37B4AEF83F8}"/>
-    <hyperlink ref="A11" r:id="rId47" display="http://www.cse.iub.edu.bd/courses/36" xr:uid="{A44925F1-78A9-43EB-A8E1-6B722B82C246}"/>
-    <hyperlink ref="B11" r:id="rId48" display="http://www.cse.iub.edu.bd/courses/36" xr:uid="{BF75BCD3-D717-4146-A332-023BFC2EA1BB}"/>
-    <hyperlink ref="A13" r:id="rId49" display="http://www.cse.iub.edu.bd/courses/37" xr:uid="{89F70F5D-EF16-4766-8376-DB39F3B8ECB0}"/>
-    <hyperlink ref="B13" r:id="rId50" display="http://www.cse.iub.edu.bd/courses/37" xr:uid="{C13AB3A1-2357-4305-B921-0346C30EC9E7}"/>
-    <hyperlink ref="A16" r:id="rId51" display="http://www.cse.iub.edu.bd/courses/39" xr:uid="{F5DD3875-92C9-4188-803B-E02FA3088CFB}"/>
-    <hyperlink ref="B16" r:id="rId52" display="http://www.cse.iub.edu.bd/courses/39" xr:uid="{EB730708-6AB5-49C8-9825-4813923EE854}"/>
-    <hyperlink ref="A18" r:id="rId53" display="http://www.cse.iub.edu.bd/courses/40" xr:uid="{1E398097-E0D1-44CC-97CE-65D70FE4CEC2}"/>
-    <hyperlink ref="B18" r:id="rId54" display="http://www.cse.iub.edu.bd/courses/40" xr:uid="{D08F1914-229E-4AFD-9C55-57D8AC233B59}"/>
-    <hyperlink ref="A22" r:id="rId55" display="http://www.cse.iub.edu.bd/courses/43" xr:uid="{C2E2E79D-78B7-4212-B0AA-38AC6D4602A8}"/>
-    <hyperlink ref="B22" r:id="rId56" display="http://www.cse.iub.edu.bd/courses/43" xr:uid="{FEE2C372-0D61-432C-9B2A-9D7324029E83}"/>
-    <hyperlink ref="A26" r:id="rId57" display="http://www.cse.iub.edu.bd/courses/46" xr:uid="{8A26AB20-D943-4550-8970-A11E148FBBF1}"/>
-    <hyperlink ref="B26" r:id="rId58" display="http://www.cse.iub.edu.bd/courses/46" xr:uid="{A1CE6EC5-F97F-484F-B58E-A30A92930BF4}"/>
-    <hyperlink ref="A28" r:id="rId59" display="http://www.cse.iub.edu.bd/courses/47" xr:uid="{AFD696B7-5067-4615-B03D-85C4BA7D9209}"/>
-    <hyperlink ref="B28" r:id="rId60" display="http://www.cse.iub.edu.bd/courses/47" xr:uid="{8FE34D0B-5063-4314-89E8-95A5BB2ED789}"/>
-    <hyperlink ref="A54" r:id="rId61" location="collapse1" display="http://slass.iub.edu.bd/english/bil.php - collapse1" xr:uid="{47FA0DA9-109B-4754-8217-D215F2CF2808}"/>
-    <hyperlink ref="A55" r:id="rId62" location="collapse2" display="http://slass.iub.edu.bd/english/bil.php - collapse2" xr:uid="{F61CA84D-EC35-4A4D-8DB0-24036AFDC076}"/>
-    <hyperlink ref="B69" r:id="rId63" display="http://phy.iub.edu.bd/course/phy201" xr:uid="{B747EE87-00F6-4910-9DEB-13D0EEE5BDBF}"/>
-    <hyperlink ref="B70" r:id="rId64" display="http://phy.iub.edu.bd/course/phy202" xr:uid="{9577248E-5543-4D85-8F33-993ED1465EE8}"/>
-    <hyperlink ref="B71" r:id="rId65" display="http://phy.iub.edu.bd/course/phy203" xr:uid="{51C5773C-F6A7-4FC9-94C5-D1882988EDFF}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId66"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Dataset complete for TechFest
</commit_message>
<xml_diff>
--- a/DataSheets/course.xlsx
+++ b/DataSheets/course.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Project_REDSight_DBMS_GROUP_1\DataSheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A07A59C-A398-46A2-A391-1D0A64EFC05F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C452A8C9-4B19-48DD-9818-B08C8FDCF543}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{45C0E8D6-B45C-4F58-8F64-0C9D44AE474B}"/>
+    <workbookView xWindow="43200" yWindow="0" windowWidth="14400" windowHeight="15750" xr2:uid="{45C0E8D6-B45C-4F58-8F64-0C9D44AE474B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -770,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A569DFA1-FE8D-4969-A877-C88B17F78045}">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D58" sqref="D58"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.28515625" defaultRowHeight="25.5" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>